<commit_message>
update nopub sched, slides, hws
</commit_message>
<xml_diff>
--- a/docs/nopublish/groups.xlsx
+++ b/docs/nopublish/groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\Intro-Data-Science\c1-intro-fall-2021\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC2556F-574D-48AF-B63A-58383EE57649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C11DC3-01A5-45C1-9694-055964B0389A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="360" windowWidth="28800" windowHeight="14985" xr2:uid="{82FEB544-DC35-4408-89F9-F4A657CE9573}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11145" xr2:uid="{82FEB544-DC35-4408-89F9-F4A657CE9573}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Manuel</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Cheng</t>
   </si>
   <si>
-    <t>Nichole</t>
-  </si>
-  <si>
-    <t>Kelly</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
@@ -103,6 +97,93 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>Claas</t>
+  </si>
+  <si>
+    <t>Cassie</t>
+  </si>
+  <si>
+    <t>Malcom</t>
+  </si>
+  <si>
+    <t>Mavis</t>
+  </si>
+  <si>
+    <t>Gallo</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t>Berny</t>
+  </si>
+  <si>
+    <t>Aubrey</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Shawn</t>
+  </si>
+  <si>
+    <t>McWeeny</t>
+  </si>
+  <si>
+    <t>Heather</t>
+  </si>
+  <si>
+    <t>Leonard</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Abbie</t>
+  </si>
+  <si>
+    <t>Sanders</t>
+  </si>
+  <si>
+    <t>Rebecca</t>
+  </si>
+  <si>
+    <t>Gordon</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Bates</t>
+  </si>
+  <si>
+    <t>Esmeralda</t>
+  </si>
+  <si>
+    <t>Castro</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Zach</t>
+  </si>
+  <si>
+    <t>Kaylor</t>
+  </si>
+  <si>
+    <t>Khurana</t>
+  </si>
+  <si>
+    <t>Adriana</t>
+  </si>
+  <si>
+    <t>Connd</t>
   </si>
 </sst>
 </file>
@@ -118,12 +199,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,8 +225,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,15 +543,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEEF4479-1AC0-4FF0-8CC8-4FD64569A518}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -492,6 +581,9 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -500,6 +592,9 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -508,77 +603,220 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>